<commit_message>
Update on 20250120 part 7
</commit_message>
<xml_diff>
--- a/IPV6直播源汇总/移动ITV-域名版.xlsx
+++ b/IPV6直播源汇总/移动ITV-域名版.xlsx
@@ -22,14 +22,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">体育!$A$1:$D$165</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">卫视!$A$1:$D$353</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$D$265</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$331</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$D$333</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5240" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5248" uniqueCount="922">
   <si>
     <t>CCTV-1</t>
   </si>
@@ -2803,6 +2803,9 @@
   <si>
     <t>id=4886720949268374180</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NewTV热播精选</t>
   </si>
 </sst>
 </file>
@@ -11762,9 +11765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection sqref="A1:D125"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -14710,11 +14711,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D331"/>
+  <dimension ref="A1:D333"/>
   <sheetViews>
-    <sheetView topLeftCell="A308" workbookViewId="0">
-      <selection sqref="A1:D331"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -18212,30 +18211,30 @@
     </row>
     <row r="250" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A250" s="2" t="s">
-        <v>278</v>
+        <v>921</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="D250" t="s">
-        <v>410</v>
+        <v>719</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A251" s="2" t="s">
-        <v>278</v>
+        <v>921</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
       <c r="D251" t="s">
-        <v>410</v>
+        <v>719</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18246,10 +18245,10 @@
         <v>29</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="D252" t="s">
-        <v>721</v>
+        <v>410</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18260,15 +18259,15 @@
         <v>29</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>105</v>
+        <v>171</v>
       </c>
       <c r="D253" t="s">
-        <v>721</v>
+        <v>410</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A254" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>29</v>
@@ -18277,12 +18276,12 @@
         <v>104</v>
       </c>
       <c r="D254" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A255" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>29</v>
@@ -18291,7 +18290,7 @@
         <v>105</v>
       </c>
       <c r="D255" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18302,10 +18301,10 @@
         <v>29</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="D256" t="s">
-        <v>411</v>
+        <v>722</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18316,38 +18315,38 @@
         <v>29</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
       <c r="D257" t="s">
-        <v>411</v>
+        <v>722</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A258" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="D258" t="s">
-        <v>723</v>
+        <v>411</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A259" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>105</v>
+        <v>171</v>
       </c>
       <c r="D259" t="s">
-        <v>723</v>
+        <v>411</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18358,10 +18357,10 @@
         <v>29</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="D260" t="s">
-        <v>412</v>
+        <v>723</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18372,10 +18371,10 @@
         <v>29</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
       <c r="D261" t="s">
-        <v>412</v>
+        <v>723</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18386,10 +18385,10 @@
         <v>29</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="D262" t="s">
-        <v>724</v>
+        <v>412</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18400,38 +18399,38 @@
         <v>29</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>105</v>
+        <v>171</v>
       </c>
       <c r="D263" t="s">
-        <v>724</v>
+        <v>412</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A264" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="D264" t="s">
-        <v>413</v>
+        <v>724</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A265" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
       <c r="D265" t="s">
-        <v>413</v>
+        <v>724</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18442,10 +18441,10 @@
         <v>29</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="D266" t="s">
-        <v>725</v>
+        <v>413</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18456,38 +18455,38 @@
         <v>29</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>105</v>
+        <v>171</v>
       </c>
       <c r="D267" t="s">
-        <v>725</v>
+        <v>413</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A268" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="D268" t="s">
-        <v>414</v>
+        <v>725</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A269" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
       <c r="D269" t="s">
-        <v>414</v>
+        <v>725</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18498,10 +18497,10 @@
         <v>29</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D270" t="s">
-        <v>776</v>
+        <v>414</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18512,38 +18511,38 @@
         <v>29</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D271" t="s">
-        <v>776</v>
+        <v>414</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A272" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D272" t="s">
-        <v>415</v>
+        <v>776</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A273" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D273" t="s">
-        <v>415</v>
+        <v>776</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18554,10 +18553,10 @@
         <v>29</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D274" t="s">
-        <v>777</v>
+        <v>415</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18568,38 +18567,38 @@
         <v>29</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D275" t="s">
-        <v>777</v>
+        <v>415</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A276" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D276" t="s">
-        <v>416</v>
+        <v>777</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A277" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D277" t="s">
-        <v>416</v>
+        <v>777</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18610,10 +18609,10 @@
         <v>29</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D278" t="s">
-        <v>778</v>
+        <v>416</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18624,43 +18623,43 @@
         <v>29</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D279" t="s">
-        <v>778</v>
+        <v>416</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A280" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B280" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D280" t="s">
-        <v>417</v>
+        <v>778</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A281" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D281" t="s">
-        <v>417</v>
+        <v>778</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A282" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>29</v>
@@ -18669,12 +18668,12 @@
         <v>170</v>
       </c>
       <c r="D282" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A283" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>29</v>
@@ -18683,7 +18682,7 @@
         <v>171</v>
       </c>
       <c r="D283" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="284" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18694,10 +18693,10 @@
         <v>29</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="D284" t="s">
-        <v>542</v>
+        <v>418</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18708,38 +18707,38 @@
         <v>29</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="D285" t="s">
-        <v>542</v>
+        <v>418</v>
       </c>
     </row>
     <row r="286" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A286" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="D286" t="s">
-        <v>419</v>
+        <v>542</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A287" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="D287" t="s">
-        <v>419</v>
+        <v>542</v>
       </c>
     </row>
     <row r="288" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18750,10 +18749,10 @@
         <v>29</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D288" t="s">
-        <v>779</v>
+        <v>419</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18764,38 +18763,38 @@
         <v>29</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D289" t="s">
-        <v>779</v>
+        <v>419</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A290" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D290" t="s">
-        <v>420</v>
+        <v>779</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A291" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D291" t="s">
-        <v>420</v>
+        <v>779</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18806,10 +18805,10 @@
         <v>29</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D292" t="s">
-        <v>780</v>
+        <v>420</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18820,15 +18819,15 @@
         <v>29</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D293" t="s">
-        <v>780</v>
+        <v>420</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A294" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>29</v>
@@ -18837,12 +18836,12 @@
         <v>163</v>
       </c>
       <c r="D294" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="295" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A295" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>29</v>
@@ -18851,35 +18850,35 @@
         <v>164</v>
       </c>
       <c r="D295" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A296" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B296" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D296" t="s">
-        <v>421</v>
+        <v>781</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A297" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D297" t="s">
-        <v>421</v>
+        <v>781</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18890,10 +18889,10 @@
         <v>29</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D298" t="s">
-        <v>782</v>
+        <v>421</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18904,38 +18903,38 @@
         <v>29</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D299" t="s">
-        <v>782</v>
+        <v>421</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A300" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D300" t="s">
-        <v>422</v>
+        <v>782</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A301" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D301" t="s">
-        <v>422</v>
+        <v>782</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18946,10 +18945,10 @@
         <v>29</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D302" t="s">
-        <v>783</v>
+        <v>422</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -18960,38 +18959,38 @@
         <v>29</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D303" t="s">
-        <v>783</v>
+        <v>422</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A304" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D304" t="s">
-        <v>423</v>
+        <v>783</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A305" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D305" t="s">
-        <v>423</v>
+        <v>783</v>
       </c>
     </row>
     <row r="306" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19002,10 +19001,10 @@
         <v>29</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D306" t="s">
-        <v>784</v>
+        <v>423</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19016,38 +19015,38 @@
         <v>29</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D307" t="s">
-        <v>784</v>
+        <v>423</v>
       </c>
     </row>
     <row r="308" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A308" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D308" t="s">
-        <v>424</v>
+        <v>784</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A309" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B309" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D309" t="s">
-        <v>424</v>
+        <v>784</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19058,10 +19057,10 @@
         <v>29</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D310" t="s">
-        <v>785</v>
+        <v>424</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19072,38 +19071,38 @@
         <v>29</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D311" t="s">
-        <v>785</v>
+        <v>424</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A312" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D312" t="s">
-        <v>425</v>
+        <v>785</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A313" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B313" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D313" t="s">
-        <v>425</v>
+        <v>785</v>
       </c>
     </row>
     <row r="314" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19114,10 +19113,10 @@
         <v>29</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D314" t="s">
-        <v>786</v>
+        <v>425</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19128,38 +19127,38 @@
         <v>29</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D315" t="s">
-        <v>786</v>
+        <v>425</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A316" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B316" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D316" t="s">
-        <v>426</v>
+        <v>786</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A317" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B317" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D317" t="s">
-        <v>426</v>
+        <v>786</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19170,10 +19169,10 @@
         <v>29</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D318" t="s">
-        <v>787</v>
+        <v>426</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19184,38 +19183,38 @@
         <v>29</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D319" t="s">
-        <v>787</v>
+        <v>426</v>
       </c>
     </row>
     <row r="320" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A320" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B320" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D320" t="s">
-        <v>427</v>
+        <v>787</v>
       </c>
     </row>
     <row r="321" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A321" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D321" t="s">
-        <v>427</v>
+        <v>787</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19226,10 +19225,10 @@
         <v>29</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D322" t="s">
-        <v>788</v>
+        <v>427</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19240,38 +19239,38 @@
         <v>29</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D323" t="s">
-        <v>788</v>
+        <v>427</v>
       </c>
     </row>
     <row r="324" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A324" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="D324" t="s">
-        <v>726</v>
+        <v>788</v>
       </c>
     </row>
     <row r="325" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A325" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="D325" t="s">
-        <v>726</v>
+        <v>788</v>
       </c>
     </row>
     <row r="326" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19282,10 +19281,10 @@
         <v>29</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="D326" t="s">
-        <v>428</v>
+        <v>726</v>
       </c>
     </row>
     <row r="327" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19296,15 +19295,15 @@
         <v>29</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
       <c r="D327" t="s">
-        <v>428</v>
+        <v>726</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A328" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B328" s="2" t="s">
         <v>29</v>
@@ -19313,12 +19312,12 @@
         <v>170</v>
       </c>
       <c r="D328" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="329" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A329" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B329" s="2" t="s">
         <v>29</v>
@@ -19327,7 +19326,7 @@
         <v>171</v>
       </c>
       <c r="D329" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19338,10 +19337,10 @@
         <v>29</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="D330" t="s">
-        <v>543</v>
+        <v>429</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
@@ -19352,14 +19351,42 @@
         <v>29</v>
       </c>
       <c r="C331" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D331" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A332" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C332" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D332" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A333" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C333" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D331" t="s">
+      <c r="D333" t="s">
         <v>543</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D331"/>
+  <autoFilter ref="A1:D333"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>